<commit_message>
New graphs for 01_LCA, with multi impact analysis
</commit_message>
<xml_diff>
--- a/files/lci_cw.xlsx
+++ b/files/lci_cw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB110D6E-11B7-42DA-8A14-CB23CF9A068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D177057-351E-4CB4-B87C-3C565214A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" firstSheet="45" activeTab="48" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" activeTab="1" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -858,9 +858,6 @@
     <t>years</t>
   </si>
   <si>
-    <t>years, lifespan of the curtain wall</t>
-  </si>
-  <si>
     <t>use of curtain wall</t>
   </si>
   <si>
@@ -1101,9 +1098,6 @@
     <t>param_elec_use</t>
   </si>
   <si>
-    <t>param_lifespan</t>
-  </si>
-  <si>
     <t>param_thermal_curtain</t>
   </si>
   <si>
@@ -1146,12 +1140,6 @@
     <t>param_dg</t>
   </si>
   <si>
-    <t>param_elec_use *  param_lifespan</t>
-  </si>
-  <si>
-    <t>param_natural_gas *  param_lifespan</t>
-  </si>
-  <si>
     <t>param_tg_2coatings_xenon</t>
   </si>
   <si>
@@ -1366,6 +1354,18 @@
   </si>
   <si>
     <t>be_market_eol_screen</t>
+  </si>
+  <si>
+    <t>years of use of the curtain wall</t>
+  </si>
+  <si>
+    <t>param_servicelife</t>
+  </si>
+  <si>
+    <t>param_elec_use *  param_servicelife</t>
+  </si>
+  <si>
+    <t>param_natural_gas *  param_servicelife</t>
   </si>
 </sst>
 </file>
@@ -2263,35 +2263,35 @@
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D36">
         <v>1500</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D37">
         <v>2700</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D38">
         <v>1500</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>103</v>
       </c>
       <c r="F49" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D51" s="13">
         <f>100/1000000*D38</f>
@@ -2438,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -2492,7 +2492,7 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>103</v>
       </c>
       <c r="F62" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D64" s="13">
         <f>100/1000000*D38</f>
@@ -2576,7 +2576,7 @@
         <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
@@ -2684,12 +2684,12 @@
         <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="27"/>
@@ -2723,7 +2723,7 @@
         <v>13</v>
       </c>
       <c r="F80" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>13</v>
       </c>
       <c r="F81" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -2780,7 +2780,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -2798,7 +2798,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -2986,7 +2986,7 @@
         <v>93</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>96</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>66</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>98</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3177,7 +3177,7 @@
         <v>100</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>102</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
     </row>
     <row r="20" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B20" s="22">
         <v>1</v>
@@ -3313,7 +3313,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O20" s="24"/>
     </row>
@@ -3356,7 +3356,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -3374,7 +3374,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -3512,7 +3512,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -3605,7 +3605,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -6292,8 +6292,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6413,7 +6413,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" t="s">
         <v>254</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
         <v>254</v>
@@ -6443,22 +6443,22 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>339</v>
+        <v>425</v>
       </c>
       <c r="B13" t="s">
         <v>257</v>
       </c>
       <c r="C13" s="41">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>258</v>
+        <v>424</v>
       </c>
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -6467,13 +6467,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -6482,13 +6482,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -6497,13 +6497,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -6512,13 +6512,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -6527,13 +6527,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O18"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -6542,13 +6542,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O19"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -6557,13 +6557,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -6572,13 +6572,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -6587,13 +6587,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -6602,13 +6602,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -6617,13 +6617,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -6632,13 +6632,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O25"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -6647,13 +6647,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O26"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -6662,13 +6662,13 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O27"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -6677,13 +6677,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -6692,13 +6692,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O30"/>
     </row>
@@ -7212,7 +7212,7 @@
     </row>
     <row r="51" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B51" s="46">
         <f>Hypothesis!D64</f>
@@ -7252,7 +7252,7 @@
         <v>64</v>
       </c>
       <c r="N51" s="35" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O51" s="45"/>
     </row>
@@ -7340,7 +7340,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -7358,7 +7358,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -7503,7 +7503,7 @@
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -7543,7 +7543,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -7720,7 +7720,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -7763,7 +7763,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -7781,7 +7781,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -7880,7 +7880,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -7919,13 +7919,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -7964,7 +7964,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -10013,7 +10013,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10031,7 +10031,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -10176,7 +10176,7 @@
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -10216,7 +10216,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -10354,7 +10354,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -10393,7 +10393,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -10436,7 +10436,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10454,7 +10454,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -10553,7 +10553,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -10592,13 +10592,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -10637,7 +10637,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -10973,7 +10973,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10991,7 +10991,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11136,7 +11136,7 @@
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -11176,7 +11176,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -11314,7 +11314,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -11353,7 +11353,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -11396,7 +11396,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -11414,7 +11414,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11513,7 +11513,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -11552,13 +11552,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -11597,7 +11597,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -11640,7 +11640,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -11658,7 +11658,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12" s="22">
         <f>Hypothesis!D43</f>
@@ -11797,7 +11797,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -11849,7 +11849,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B14" s="42">
         <f>B13</f>
@@ -11889,7 +11889,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
     </row>
     <row r="18" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B18" s="22">
         <v>1</v>
@@ -12065,7 +12065,7 @@
         <v>64</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O18" s="24"/>
     </row>
@@ -12108,7 +12108,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12126,7 +12126,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12225,7 +12225,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -12264,13 +12264,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -12309,7 +12309,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -12352,7 +12352,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12370,7 +12370,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12515,7 +12515,7 @@
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -12555,7 +12555,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -12693,7 +12693,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -12732,7 +12732,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -12773,7 +12773,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12791,7 +12791,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12890,7 +12890,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -12929,13 +12929,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -12974,7 +12974,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -13686,7 +13686,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -13704,7 +13704,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -13941,7 +13941,7 @@
     </row>
     <row r="15" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B15" s="42">
         <f>B14</f>
@@ -13981,7 +13981,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -14118,7 +14118,7 @@
     </row>
     <row r="19" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B19" s="22">
         <v>1</v>
@@ -14157,7 +14157,7 @@
         <v>64</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O19" s="24"/>
     </row>
@@ -14203,7 +14203,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -14221,7 +14221,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -14320,7 +14320,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -14359,13 +14359,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -14404,7 +14404,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -16603,7 +16603,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16635,7 +16635,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -16651,7 +16651,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -16749,7 +16749,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B12" s="40">
         <v>-1</v>
@@ -16759,7 +16759,7 @@
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -16789,7 +16789,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -16803,7 +16803,7 @@
         <v>72</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>71</v>
@@ -16851,7 +16851,7 @@
         <v>72</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>71</v>
@@ -16899,7 +16899,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>71</v>
@@ -16946,7 +16946,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>71</v>
@@ -16993,7 +16993,7 @@
         <v>72</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>71</v>
@@ -17040,7 +17040,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>71</v>
@@ -17078,7 +17078,7 @@
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -17087,7 +17087,7 @@
         <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>71</v>
@@ -17120,7 +17120,7 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -17134,7 +17134,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>71</v>
@@ -17181,7 +17181,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>71</v>
@@ -17228,7 +17228,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>71</v>
@@ -17266,7 +17266,7 @@
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -17275,7 +17275,7 @@
         <v>72</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>71</v>
@@ -17308,12 +17308,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -17322,7 +17322,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>71</v>
@@ -17355,12 +17355,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -17369,7 +17369,7 @@
         <v>72</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>71</v>
@@ -17402,12 +17402,12 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
@@ -17416,7 +17416,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>71</v>
@@ -17449,7 +17449,7 @@
         <v>64</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -17463,7 +17463,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>71</v>
@@ -17501,7 +17501,7 @@
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B28" s="40">
         <v>0</v>
@@ -17510,7 +17510,7 @@
         <v>72</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>71</v>
@@ -17543,7 +17543,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -17557,7 +17557,7 @@
         <v>62</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>354</v>
+        <v>426</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>63</v>
@@ -17604,7 +17604,7 @@
         <v>247</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>63</v>
@@ -17642,7 +17642,7 @@
     </row>
     <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B31" s="40">
         <v>1</v>
@@ -17682,7 +17682,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P31" s="24"/>
     </row>
@@ -17728,7 +17728,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -17744,7 +17744,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -17842,7 +17842,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B12" s="40">
         <v>1</v>
@@ -17882,12 +17882,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B13" s="40">
         <v>-1</v>
@@ -17897,7 +17897,7 @@
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -17927,7 +17927,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -17972,7 +17972,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -17988,7 +17988,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -18095,7 +18095,7 @@
         <v>72</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>71</v>
@@ -18143,7 +18143,7 @@
         <v>72</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>71</v>
@@ -18191,7 +18191,7 @@
         <v>72</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>71</v>
@@ -18238,7 +18238,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>71</v>
@@ -18285,7 +18285,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>71</v>
@@ -18332,7 +18332,7 @@
         <v>72</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>71</v>
@@ -18370,7 +18370,7 @@
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -18379,7 +18379,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>71</v>
@@ -18412,7 +18412,7 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -18426,7 +18426,7 @@
         <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>71</v>
@@ -18473,7 +18473,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>71</v>
@@ -18520,7 +18520,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>71</v>
@@ -18558,7 +18558,7 @@
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -18567,7 +18567,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>71</v>
@@ -18600,12 +18600,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -18614,7 +18614,7 @@
         <v>72</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>71</v>
@@ -18647,12 +18647,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -18661,7 +18661,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>71</v>
@@ -18694,12 +18694,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -18708,7 +18708,7 @@
         <v>72</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>71</v>
@@ -18741,7 +18741,7 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -18755,7 +18755,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>71</v>
@@ -18793,7 +18793,7 @@
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B27" s="40">
         <v>0</v>
@@ -18802,7 +18802,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>71</v>
@@ -18835,12 +18835,12 @@
         <v>64</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B28" s="40">
         <v>1</v>
@@ -18880,7 +18880,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P28" s="24"/>
     </row>
@@ -18924,7 +18924,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -18940,7 +18940,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -19078,12 +19078,12 @@
         <v>108</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B13" s="46">
         <f>Hypothesis!D38*(Hypothesis!D32*2+Hypothesis!D33*2)*100/1000000/Hypothesis!D31</f>
@@ -19123,15 +19123,15 @@
         <v>64</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B14" s="46">
         <f>-B12-B13</f>
@@ -19171,15 +19171,15 @@
         <v>64</v>
       </c>
       <c r="N14" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="O14" s="45" t="s">
         <v>377</v>
-      </c>
-      <c r="O14" s="45" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B15" s="40">
         <v>1</v>
@@ -19218,7 +19218,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O15" s="24"/>
     </row>
@@ -19233,7 +19233,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19265,7 +19265,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19281,7 +19281,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -19388,7 +19388,7 @@
         <v>62</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>354</v>
+        <v>426</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>63</v>
@@ -19435,7 +19435,7 @@
         <v>247</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>63</v>
@@ -19473,7 +19473,7 @@
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B14" s="40">
         <v>1</v>
@@ -19513,7 +19513,7 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P14" s="24"/>
     </row>
@@ -19526,7 +19526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F3D49-74C2-4BFC-A6B6-5745C01BC058}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+    <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -19559,7 +19559,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19575,7 +19575,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -19673,7 +19673,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -19682,10 +19682,10 @@
         <v>72</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -19715,12 +19715,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -19729,10 +19729,10 @@
         <v>72</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -19762,12 +19762,12 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -19776,10 +19776,10 @@
         <v>72</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>64</v>
@@ -19809,12 +19809,12 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -19823,10 +19823,10 @@
         <v>72</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>64</v>
@@ -19856,12 +19856,12 @@
         <v>64</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B16" s="40">
         <v>0</v>
@@ -19870,10 +19870,10 @@
         <v>72</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>64</v>
@@ -19903,12 +19903,12 @@
         <v>64</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B17" s="40">
         <v>0</v>
@@ -19917,10 +19917,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>64</v>
@@ -19950,12 +19950,12 @@
         <v>64</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -19964,10 +19964,10 @@
         <v>72</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>64</v>
@@ -19997,12 +19997,12 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -20011,10 +20011,10 @@
         <v>72</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>64</v>
@@ -20044,12 +20044,12 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -20058,10 +20058,10 @@
         <v>72</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>64</v>
@@ -20091,12 +20091,12 @@
         <v>64</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -20105,10 +20105,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>64</v>
@@ -20138,12 +20138,12 @@
         <v>64</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -20152,10 +20152,10 @@
         <v>72</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>64</v>
@@ -20185,12 +20185,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -20199,10 +20199,10 @@
         <v>72</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>64</v>
@@ -20232,12 +20232,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -20246,10 +20246,10 @@
         <v>72</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>64</v>
@@ -20279,12 +20279,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -20293,10 +20293,10 @@
         <v>72</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>64</v>
@@ -20326,12 +20326,12 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
@@ -20340,10 +20340,10 @@
         <v>72</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>64</v>
@@ -20373,12 +20373,12 @@
         <v>64</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B27" s="40">
         <v>1</v>
@@ -20418,7 +20418,7 @@
         <v>64</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="P27" s="24"/>
     </row>
@@ -21247,7 +21247,7 @@
     </row>
     <row r="20" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B20" s="46">
         <f>Hypothesis!D51</f>
@@ -21287,7 +21287,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="35" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O20" s="45"/>
     </row>

</xml_diff>

<commit_message>
Weighted impact calculation and analysis added to 02_LCA
</commit_message>
<xml_diff>
--- a/files/lci_cw.xlsx
+++ b/files/lci_cw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D177057-351E-4CB4-B87C-3C565214A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236D717C-7544-4DCC-96E0-183538B7EDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" activeTab="1" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" firstSheet="26" activeTab="31" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -522,9 +522,6 @@
     <t>1dace3ae96abb71bab013d0fc90b3e3a</t>
   </si>
   <si>
-    <t>LCI according to oekobaudat, "Modular Automatic Drive System for Sliding Doors in the ES 200 product family", adapted to screens. Total weight = 6kg per unit of screen instead of 30kg.</t>
-  </si>
-  <si>
     <t>market for screen, metalised blind fabric</t>
   </si>
   <si>
@@ -1366,6 +1363,9 @@
   </si>
   <si>
     <t>param_natural_gas *  param_servicelife</t>
+  </si>
+  <si>
+    <t>LCI according to oekobaudat, "Modular Automatic Drive System for Sliding Doors in the ES 200 product family", adapted to screens. Total weight = 3kg per unit of screen instead of 30kg.</t>
   </si>
 </sst>
 </file>
@@ -1937,8 +1937,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,35 +2263,35 @@
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D36">
         <v>1500</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D37">
         <v>2700</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D38">
         <v>1500</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>103</v>
       </c>
       <c r="F49" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D51" s="13">
         <f>100/1000000*D38</f>
@@ -2438,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -2492,7 +2492,7 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>103</v>
       </c>
       <c r="F62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D64" s="13">
         <f>100/1000000*D38</f>
@@ -2576,7 +2576,7 @@
         <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
@@ -2684,12 +2684,12 @@
         <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="27"/>
@@ -2723,7 +2723,7 @@
         <v>13</v>
       </c>
       <c r="F80" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>13</v>
       </c>
       <c r="F81" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -2780,7 +2780,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -2798,7 +2798,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -2907,7 +2907,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>64</v>
@@ -2937,7 +2937,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O12" s="32"/>
     </row>
@@ -2986,7 +2986,7 @@
         <v>93</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>96</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>66</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>98</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3177,7 +3177,7 @@
         <v>100</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>102</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
     </row>
     <row r="20" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="22">
         <v>1</v>
@@ -3313,7 +3313,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O20" s="24"/>
     </row>
@@ -3356,7 +3356,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -3374,7 +3374,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -3512,7 +3512,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -3605,7 +3605,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -3649,7 +3649,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -3806,13 +3806,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="18">
         <v>0.95</v>
@@ -3851,7 +3851,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3988,7 +3988,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -4027,7 +4027,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -4071,7 +4071,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -4089,7 +4089,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -4227,13 +4227,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -4272,7 +4272,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -4316,7 +4316,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -4334,7 +4334,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -4473,13 +4473,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13" s="18">
         <v>0.95</v>
@@ -4518,7 +4518,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -4655,7 +4655,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -4694,7 +4694,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -4736,7 +4736,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -4754,7 +4754,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -4892,13 +4892,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -4937,7 +4937,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -4981,7 +4981,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -4999,7 +4999,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -5138,7 +5138,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -5184,7 +5184,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -5322,7 +5322,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -5361,7 +5361,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -5408,7 +5408,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -5426,7 +5426,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -5564,13 +5564,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -5609,7 +5609,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -5653,7 +5653,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -5671,7 +5671,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -5810,13 +5810,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -5856,7 +5856,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -6033,7 +6033,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -6077,7 +6077,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -6095,7 +6095,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -6194,7 +6194,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -6233,13 +6233,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -6278,7 +6278,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -6292,8 +6292,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6351,7 +6351,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O6"/>
     </row>
@@ -6366,10 +6366,10 @@
         <v>52</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -6383,7 +6383,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C9" s="39"/>
       <c r="O9"/>
@@ -6399,10 +6399,10 @@
         <v>52</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
@@ -6413,52 +6413,52 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="41">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="41">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="41">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -6467,13 +6467,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -6482,13 +6482,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -6497,13 +6497,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -6512,13 +6512,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -6527,13 +6527,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O18"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -6542,13 +6542,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O19"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -6557,13 +6557,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -6572,13 +6572,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -6587,13 +6587,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -6602,13 +6602,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -6617,13 +6617,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -6632,13 +6632,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O25"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -6647,13 +6647,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O26"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -6662,13 +6662,13 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O27"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -6677,13 +6677,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -6692,13 +6692,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O30"/>
     </row>
@@ -6738,7 +6738,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="17"/>
@@ -6780,7 +6780,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -6847,7 +6847,7 @@
         <v>49</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" s="23" t="s">
         <v>64</v>
@@ -6877,7 +6877,7 @@
         <v>64</v>
       </c>
       <c r="N43" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O43" s="32"/>
     </row>
@@ -7212,7 +7212,7 @@
     </row>
     <row r="51" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B51" s="46">
         <f>Hypothesis!D64</f>
@@ -7252,7 +7252,7 @@
         <v>64</v>
       </c>
       <c r="N51" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O51" s="45"/>
     </row>
@@ -7297,7 +7297,7 @@
         <v>64</v>
       </c>
       <c r="N52" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O52" s="24"/>
     </row>
@@ -7340,7 +7340,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -7358,7 +7358,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -7497,13 +7497,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -7543,7 +7543,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -7720,7 +7720,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -7763,7 +7763,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -7781,7 +7781,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -7880,7 +7880,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -7919,13 +7919,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -7964,7 +7964,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -8008,7 +8008,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -8026,7 +8026,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -8165,13 +8165,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -8211,7 +8211,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -8348,7 +8348,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -8387,7 +8387,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -8431,7 +8431,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -8449,7 +8449,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -8491,7 +8491,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -8548,7 +8548,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -8587,13 +8587,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -8632,7 +8632,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -8676,7 +8676,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -8694,7 +8694,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -8833,13 +8833,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -8879,7 +8879,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -9017,7 +9017,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -9056,7 +9056,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -9100,7 +9100,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -9118,7 +9118,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -9217,7 +9217,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -9256,13 +9256,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -9301,7 +9301,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -9345,7 +9345,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -9363,7 +9363,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -9502,13 +9502,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -9548,7 +9548,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -9725,7 +9725,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -9769,7 +9769,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -9787,7 +9787,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -9886,7 +9886,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -9925,13 +9925,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -9970,7 +9970,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -10013,7 +10013,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10031,7 +10031,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -10170,13 +10170,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -10216,7 +10216,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -10354,7 +10354,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -10393,7 +10393,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -10436,7 +10436,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10454,7 +10454,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -10553,7 +10553,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -10592,13 +10592,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -10637,7 +10637,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -10699,7 +10699,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -10837,7 +10837,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -10930,7 +10930,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -10973,7 +10973,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -10991,7 +10991,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11130,13 +11130,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -11176,7 +11176,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -11314,7 +11314,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -11353,7 +11353,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -11396,7 +11396,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -11414,7 +11414,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11513,7 +11513,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -11552,13 +11552,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -11597,7 +11597,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -11610,8 +11610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E1620C-AF18-4A30-94EC-3B2E34B9A5F9}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11640,7 +11640,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -11658,7 +11658,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B12" s="22">
         <f>Hypothesis!D43</f>
@@ -11797,13 +11797,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -11843,13 +11843,13 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B14" s="42">
         <f>B13</f>
@@ -11889,7 +11889,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -12026,7 +12026,7 @@
     </row>
     <row r="18" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B18" s="22">
         <v>1</v>
@@ -12065,7 +12065,7 @@
         <v>64</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O18" s="24"/>
     </row>
@@ -12108,7 +12108,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12126,7 +12126,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12225,7 +12225,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -12264,13 +12264,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -12309,7 +12309,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -12352,7 +12352,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12370,7 +12370,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12509,13 +12509,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -12555,7 +12555,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -12693,7 +12693,7 @@
     </row>
     <row r="17" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -12732,7 +12732,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -12773,7 +12773,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -12791,7 +12791,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -12890,7 +12890,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -12929,13 +12929,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -12974,7 +12974,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -13036,7 +13036,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -13175,13 +13175,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" s="22">
         <f>Hypothesis!D42</f>
@@ -13221,7 +13221,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O13" s="32"/>
     </row>
@@ -13398,7 +13398,7 @@
         <v>64</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O17" s="24"/>
     </row>
@@ -13442,7 +13442,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -13460,7 +13460,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -13598,13 +13598,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -13643,7 +13643,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -13686,7 +13686,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -13704,7 +13704,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -13843,7 +13843,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -13889,13 +13889,13 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O13" s="24"/>
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B14" s="22">
         <f>Hypothesis!D42</f>
@@ -13935,13 +13935,13 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O14" s="32"/>
     </row>
     <row r="15" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B15" s="42">
         <f>B14</f>
@@ -13981,7 +13981,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -14118,7 +14118,7 @@
     </row>
     <row r="19" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" s="22">
         <v>1</v>
@@ -14157,7 +14157,7 @@
         <v>64</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O19" s="24"/>
     </row>
@@ -14203,7 +14203,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -14221,7 +14221,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -14320,7 +14320,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -14359,13 +14359,13 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -14404,7 +14404,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O13" s="24"/>
     </row>
@@ -14466,7 +14466,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -14575,7 +14575,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>64</v>
@@ -14605,7 +14605,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O12" s="32"/>
     </row>
@@ -14979,7 +14979,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O20" s="24"/>
     </row>
@@ -14994,7 +14994,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15041,7 +15041,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -15086,7 +15086,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -15438,7 +15438,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>64</v>
@@ -15468,7 +15468,7 @@
         <v>64</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O18" s="32"/>
     </row>
@@ -15477,8 +15477,8 @@
         <v>140</v>
       </c>
       <c r="B19" s="25">
-        <f>0.23*6/Hypothesis!D34</f>
-        <v>0.41379310344827597</v>
+        <f>0.23*3/Hypothesis!D34</f>
+        <v>0.20689655172413798</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>49</v>
@@ -15517,7 +15517,7 @@
         <v>141</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>146</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -15525,14 +15525,14 @@
         <v>75</v>
       </c>
       <c r="B20" s="22">
-        <f>0.5*6/Hypothesis!D34</f>
-        <v>0.89955022488755632</v>
+        <f>0.5*3/Hypothesis!D34</f>
+        <v>0.44977511244377816</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>64</v>
@@ -15562,7 +15562,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O20" s="32" t="s">
         <v>139</v>
@@ -15573,8 +15573,8 @@
         <v>142</v>
       </c>
       <c r="B21" s="25">
-        <f>0.23*6/Hypothesis!D34</f>
-        <v>0.41379310344827597</v>
+        <f>0.23*3/Hypothesis!D34</f>
+        <v>0.20689655172413798</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>49</v>
@@ -15613,7 +15613,7 @@
         <v>143</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>146</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -15621,8 +15621,8 @@
         <v>144</v>
       </c>
       <c r="B22" s="25">
-        <f>0.04*6/Hypothesis!D34</f>
-        <v>7.1964017991004506E-2</v>
+        <f>0.04*3/Hypothesis!D34</f>
+        <v>3.5982008995502253E-2</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>49</v>
@@ -15661,7 +15661,7 @@
         <v>145</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>146</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -15705,7 +15705,7 @@
         <v>64</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O23" s="24"/>
     </row>
@@ -15755,7 +15755,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -15773,7 +15773,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -15911,7 +15911,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -15962,7 +15962,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -16001,7 +16001,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -16045,7 +16045,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -16063,7 +16063,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -16108,7 +16108,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -16165,7 +16165,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" s="31">
         <v>0.1</v>
@@ -16204,10 +16204,10 @@
         <v>64</v>
       </c>
       <c r="N12" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -16259,7 +16259,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -16298,7 +16298,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -16343,7 +16343,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="17"/>
@@ -16361,7 +16361,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -16460,7 +16460,7 @@
     </row>
     <row r="12" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="22">
         <v>1</v>
@@ -16499,7 +16499,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -16550,7 +16550,7 @@
     </row>
     <row r="14" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -16589,7 +16589,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -16635,7 +16635,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -16651,7 +16651,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -16708,7 +16708,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>53</v>
@@ -16749,7 +16749,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B12" s="40">
         <v>-1</v>
@@ -16759,7 +16759,7 @@
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -16789,12 +16789,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -16803,7 +16803,7 @@
         <v>72</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>71</v>
@@ -16836,13 +16836,13 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -16851,7 +16851,7 @@
         <v>72</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>71</v>
@@ -16884,13 +16884,13 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -16899,7 +16899,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>71</v>
@@ -16932,12 +16932,12 @@
         <v>64</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" s="40">
         <v>0</v>
@@ -16946,7 +16946,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>71</v>
@@ -16979,12 +16979,12 @@
         <v>64</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="40">
         <v>0</v>
@@ -16993,7 +16993,7 @@
         <v>72</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>71</v>
@@ -17026,12 +17026,12 @@
         <v>64</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -17040,7 +17040,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>71</v>
@@ -17073,12 +17073,12 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -17087,7 +17087,7 @@
         <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>71</v>
@@ -17120,12 +17120,12 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -17134,7 +17134,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>71</v>
@@ -17167,12 +17167,12 @@
         <v>64</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -17181,7 +17181,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>71</v>
@@ -17214,12 +17214,12 @@
         <v>64</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -17228,7 +17228,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>71</v>
@@ -17261,12 +17261,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -17275,7 +17275,7 @@
         <v>72</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>71</v>
@@ -17308,12 +17308,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -17322,7 +17322,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>71</v>
@@ -17355,12 +17355,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -17369,7 +17369,7 @@
         <v>72</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>71</v>
@@ -17402,12 +17402,12 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
@@ -17416,7 +17416,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>71</v>
@@ -17449,12 +17449,12 @@
         <v>64</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="40">
         <v>0</v>
@@ -17463,7 +17463,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>71</v>
@@ -17496,12 +17496,12 @@
         <v>64</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B28" s="40">
         <v>0</v>
@@ -17510,7 +17510,7 @@
         <v>72</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>71</v>
@@ -17543,12 +17543,12 @@
         <v>64</v>
       </c>
       <c r="O28" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B29" s="41">
         <v>0</v>
@@ -17557,7 +17557,7 @@
         <v>62</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>63</v>
@@ -17590,21 +17590,21 @@
         <v>64</v>
       </c>
       <c r="O29" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B30" s="41">
         <v>0</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>63</v>
@@ -17613,7 +17613,7 @@
         <v>64</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>65</v>
@@ -17637,12 +17637,12 @@
         <v>64</v>
       </c>
       <c r="O30" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B31" s="40">
         <v>1</v>
@@ -17682,7 +17682,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P31" s="24"/>
     </row>
@@ -17728,7 +17728,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -17744,7 +17744,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -17801,7 +17801,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>53</v>
@@ -17842,7 +17842,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B12" s="40">
         <v>1</v>
@@ -17882,12 +17882,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B13" s="40">
         <v>-1</v>
@@ -17897,7 +17897,7 @@
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -17927,7 +17927,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -17972,7 +17972,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -17988,7 +17988,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -18045,7 +18045,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>53</v>
@@ -18086,7 +18086,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -18095,7 +18095,7 @@
         <v>72</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>71</v>
@@ -18128,13 +18128,13 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P12" s="24"/>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -18143,7 +18143,7 @@
         <v>72</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>71</v>
@@ -18176,13 +18176,13 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -18191,7 +18191,7 @@
         <v>72</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>71</v>
@@ -18224,12 +18224,12 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -18238,7 +18238,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>71</v>
@@ -18271,12 +18271,12 @@
         <v>64</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="40">
         <v>0</v>
@@ -18285,7 +18285,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>71</v>
@@ -18318,12 +18318,12 @@
         <v>64</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="40">
         <v>0</v>
@@ -18332,7 +18332,7 @@
         <v>72</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>71</v>
@@ -18365,12 +18365,12 @@
         <v>64</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -18379,7 +18379,7 @@
         <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>71</v>
@@ -18412,12 +18412,12 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -18426,7 +18426,7 @@
         <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>71</v>
@@ -18459,12 +18459,12 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -18473,7 +18473,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>71</v>
@@ -18506,12 +18506,12 @@
         <v>64</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -18520,7 +18520,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>71</v>
@@ -18553,12 +18553,12 @@
         <v>64</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -18567,7 +18567,7 @@
         <v>72</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>71</v>
@@ -18600,12 +18600,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -18614,7 +18614,7 @@
         <v>72</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>71</v>
@@ -18647,12 +18647,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -18661,7 +18661,7 @@
         <v>72</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>71</v>
@@ -18694,12 +18694,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -18708,7 +18708,7 @@
         <v>72</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>71</v>
@@ -18741,12 +18741,12 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
@@ -18755,7 +18755,7 @@
         <v>72</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>71</v>
@@ -18788,12 +18788,12 @@
         <v>64</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B27" s="40">
         <v>0</v>
@@ -18802,7 +18802,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>71</v>
@@ -18835,12 +18835,12 @@
         <v>64</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B28" s="40">
         <v>1</v>
@@ -18880,7 +18880,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P28" s="24"/>
     </row>
@@ -18924,7 +18924,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -18940,7 +18940,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -19078,12 +19078,12 @@
         <v>108</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B13" s="46">
         <f>Hypothesis!D38*(Hypothesis!D32*2+Hypothesis!D33*2)*100/1000000/Hypothesis!D31</f>
@@ -19123,15 +19123,15 @@
         <v>64</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14" s="46">
         <f>-B12-B13</f>
@@ -19147,7 +19147,7 @@
         <v>64</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G14" s="35" t="s">
         <v>65</v>
@@ -19171,15 +19171,15 @@
         <v>64</v>
       </c>
       <c r="N14" s="35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B15" s="40">
         <v>1</v>
@@ -19218,7 +19218,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O15" s="24"/>
     </row>
@@ -19265,7 +19265,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19281,7 +19281,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -19338,7 +19338,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>53</v>
@@ -19379,7 +19379,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="41">
         <v>0</v>
@@ -19388,7 +19388,7 @@
         <v>62</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>63</v>
@@ -19421,21 +19421,21 @@
         <v>64</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13" s="41">
         <v>0</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>63</v>
@@ -19444,7 +19444,7 @@
         <v>64</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>65</v>
@@ -19468,12 +19468,12 @@
         <v>64</v>
       </c>
       <c r="O13" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B14" s="40">
         <v>1</v>
@@ -19513,7 +19513,7 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P14" s="24"/>
     </row>
@@ -19559,7 +19559,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19575,7 +19575,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -19632,7 +19632,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>53</v>
@@ -19673,7 +19673,7 @@
     </row>
     <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -19682,10 +19682,10 @@
         <v>72</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>64</v>
@@ -19715,12 +19715,12 @@
         <v>64</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -19729,10 +19729,10 @@
         <v>72</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>64</v>
@@ -19762,12 +19762,12 @@
         <v>64</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -19776,10 +19776,10 @@
         <v>72</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>64</v>
@@ -19809,12 +19809,12 @@
         <v>64</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -19823,10 +19823,10 @@
         <v>72</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F15" s="23" t="s">
         <v>64</v>
@@ -19856,12 +19856,12 @@
         <v>64</v>
       </c>
       <c r="O15" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B16" s="40">
         <v>0</v>
@@ -19870,10 +19870,10 @@
         <v>72</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F16" s="23" t="s">
         <v>64</v>
@@ -19903,12 +19903,12 @@
         <v>64</v>
       </c>
       <c r="O16" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B17" s="40">
         <v>0</v>
@@ -19917,10 +19917,10 @@
         <v>72</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>64</v>
@@ -19950,12 +19950,12 @@
         <v>64</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B18" s="40">
         <v>0</v>
@@ -19964,10 +19964,10 @@
         <v>72</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>64</v>
@@ -19997,12 +19997,12 @@
         <v>64</v>
       </c>
       <c r="O18" s="23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B19" s="40">
         <v>0</v>
@@ -20011,10 +20011,10 @@
         <v>72</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>64</v>
@@ -20044,12 +20044,12 @@
         <v>64</v>
       </c>
       <c r="O19" s="23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -20058,10 +20058,10 @@
         <v>72</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>64</v>
@@ -20091,12 +20091,12 @@
         <v>64</v>
       </c>
       <c r="O20" s="23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -20105,10 +20105,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>64</v>
@@ -20138,12 +20138,12 @@
         <v>64</v>
       </c>
       <c r="O21" s="23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -20152,10 +20152,10 @@
         <v>72</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>64</v>
@@ -20185,12 +20185,12 @@
         <v>64</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -20199,10 +20199,10 @@
         <v>72</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>64</v>
@@ -20232,12 +20232,12 @@
         <v>64</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -20246,10 +20246,10 @@
         <v>72</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>64</v>
@@ -20279,12 +20279,12 @@
         <v>64</v>
       </c>
       <c r="O24" s="23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B25" s="40">
         <v>0</v>
@@ -20293,10 +20293,10 @@
         <v>72</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>64</v>
@@ -20326,12 +20326,12 @@
         <v>64</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B26" s="40">
         <v>0</v>
@@ -20340,10 +20340,10 @@
         <v>72</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>64</v>
@@ -20373,12 +20373,12 @@
         <v>64</v>
       </c>
       <c r="O26" s="23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B27" s="40">
         <v>1</v>
@@ -20418,7 +20418,7 @@
         <v>64</v>
       </c>
       <c r="O27" s="23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="P27" s="24"/>
     </row>
@@ -20480,7 +20480,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -20618,7 +20618,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -20711,7 +20711,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -20773,7 +20773,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -20882,7 +20882,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>64</v>
@@ -20912,7 +20912,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O12" s="32"/>
     </row>
@@ -21247,7 +21247,7 @@
     </row>
     <row r="20" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B20" s="46">
         <f>Hypothesis!D51</f>
@@ -21287,7 +21287,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="35" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O20" s="45"/>
     </row>
@@ -21332,7 +21332,7 @@
         <v>64</v>
       </c>
       <c r="N21" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O21" s="24"/>
     </row>
@@ -21394,7 +21394,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -21532,7 +21532,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -21625,7 +21625,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O14" s="24"/>
     </row>
@@ -21687,7 +21687,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -21796,7 +21796,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>64</v>
@@ -21826,7 +21826,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O12" s="32"/>
     </row>
@@ -22200,7 +22200,7 @@
         <v>64</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O20" s="24"/>
     </row>
@@ -22260,7 +22260,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="17"/>
@@ -22398,7 +22398,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O12" s="24"/>
     </row>
@@ -22491,7 +22491,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O14" s="24"/>
     </row>

</xml_diff>

<commit_message>
Sensitivity analysis: energy mix. Last section in 02_LCA
</commit_message>
<xml_diff>
--- a/files/lci_cw.xlsx
+++ b/files/lci_cw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236D717C-7544-4DCC-96E0-183538B7EDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F878C0A-EA0A-4119-BE61-EAAC5D547C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" firstSheet="26" activeTab="31" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="828" firstSheet="40" activeTab="48" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,12 @@
     <sheet name="Screen_Metallised_Fabric_Market" sheetId="35" r:id="rId41"/>
     <sheet name="Thermal_Curtain_Prod" sheetId="36" r:id="rId42"/>
     <sheet name="Thermal_Curtain_Market" sheetId="37" r:id="rId43"/>
-    <sheet name="CW_Prod_and_Use" sheetId="41" r:id="rId44"/>
-    <sheet name="CW_Dismantling" sheetId="59" r:id="rId45"/>
-    <sheet name="CW_Production" sheetId="42" r:id="rId46"/>
-    <sheet name="CW_Maintenance" sheetId="58" r:id="rId47"/>
-    <sheet name="CW_UsePhase_only" sheetId="43" r:id="rId48"/>
-    <sheet name="CW_EndOfLife" sheetId="60" r:id="rId49"/>
+    <sheet name="CW_Dismantling" sheetId="59" r:id="rId44"/>
+    <sheet name="CW_Production" sheetId="42" r:id="rId45"/>
+    <sheet name="CW_Maintenance" sheetId="58" r:id="rId46"/>
+    <sheet name="CW_UsePhase_only" sheetId="43" r:id="rId47"/>
+    <sheet name="CW_EndOfLife" sheetId="60" r:id="rId48"/>
+    <sheet name="CW_Prod_and_Use" sheetId="41" r:id="rId49"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5207" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4999" uniqueCount="432">
   <si>
     <t>skip</t>
   </si>
@@ -1353,9 +1353,6 @@
     <t>be_market_eol_screen</t>
   </si>
   <si>
-    <t>years of use of the curtain wall</t>
-  </si>
-  <si>
     <t>param_servicelife</t>
   </si>
   <si>
@@ -1366,6 +1363,21 @@
   </si>
   <si>
     <t>LCI according to oekobaudat, "Modular Automatic Drive System for Sliding Doors in the ES 200 product family", adapted to screens. Total weight = 3kg per unit of screen instead of 30kg.</t>
+  </si>
+  <si>
+    <t>param_elec_use *  param_lifespan</t>
+  </si>
+  <si>
+    <t>param_natural_gas *  param_lifespan</t>
+  </si>
+  <si>
+    <t>param_lifespan</t>
+  </si>
+  <si>
+    <t>1 year of use of the curtain wall</t>
+  </si>
+  <si>
+    <t>40 years of use of the curtain wall</t>
   </si>
 </sst>
 </file>
@@ -6290,10 +6302,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F331A97-D360-4614-930F-5E821087FA83}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6443,7 +6455,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B13" t="s">
         <v>256</v>
@@ -6452,28 +6464,28 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="C14" s="41">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>260</v>
+        <v>431</v>
       </c>
       <c r="O14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -6482,13 +6494,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>409</v>
+        <v>260</v>
       </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>337</v>
+        <v>408</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -6497,13 +6509,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>261</v>
+        <v>409</v>
       </c>
       <c r="O16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -6512,13 +6524,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -6527,13 +6539,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O18"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -6542,13 +6554,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O19"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -6557,13 +6569,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -6572,13 +6584,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -6587,13 +6599,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="O22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -6602,13 +6614,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -6617,13 +6629,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -6632,13 +6644,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="O25"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -6647,13 +6659,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O26"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -6662,13 +6674,13 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="O27"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -6677,13 +6689,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -6692,13 +6704,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>269</v>
+        <v>319</v>
       </c>
       <c r="O29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -6707,237 +6719,205 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
+        <v>269</v>
+      </c>
+      <c r="O30"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="41">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
         <v>334</v>
       </c>
-      <c r="O30"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C31" s="41"/>
       <c r="O31"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="41"/>
+      <c r="O32"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B34" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="17"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="C37" s="4"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+    <row r="42" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+    <row r="43" spans="1:15" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B43" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C43" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D43" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="38" t="s">
+      <c r="E43" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="38" t="s">
+      <c r="F43" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="38" t="s">
+      <c r="G43" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H43" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="I42" s="19" t="s">
+      <c r="I43" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="J43" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K43" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="L43" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M42" s="19" t="s">
+      <c r="M43" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="N42" s="19" t="s">
+      <c r="N43" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="O42" s="20" t="s">
+      <c r="O43" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+    <row r="44" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="47">
+      <c r="B44" s="47">
         <f>Hypothesis!D61</f>
         <v>3.4749000000000008</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C44" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D44" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="23" t="s">
+      <c r="E44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G43" s="23" t="s">
+      <c r="G44" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N43" s="23" t="s">
+      <c r="H44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M44" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N44" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="O43" s="32"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="46">
-        <f>B43*0.95</f>
-        <v>3.3011550000000005</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M44" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N44" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="O44" s="11" t="s">
-        <v>94</v>
-      </c>
+      <c r="O44" s="32"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B45" s="46">
-        <v>0.95</v>
+        <f>B44*0.95</f>
+        <v>3.3011550000000005</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>63</v>
@@ -6970,7 +6950,7 @@
         <v>64</v>
       </c>
       <c r="N45" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O45" s="11" t="s">
         <v>94</v>
@@ -6978,13 +6958,13 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B46" s="46">
-        <v>0.27</v>
+        <v>0.95</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>63</v>
@@ -6993,7 +6973,7 @@
         <v>64</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>65</v>
@@ -7017,7 +6997,7 @@
         <v>64</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="O46" s="11" t="s">
         <v>94</v>
@@ -7025,13 +7005,13 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B47" s="46">
-        <v>0.03</v>
+        <v>0.27</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>63</v>
@@ -7040,7 +7020,7 @@
         <v>64</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>65</v>
@@ -7064,7 +7044,7 @@
         <v>64</v>
       </c>
       <c r="N47" s="13" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="O47" s="11" t="s">
         <v>94</v>
@@ -7072,10 +7052,9 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B48" s="46">
-        <f>B47</f>
         <v>0.03</v>
       </c>
       <c r="C48" s="11" t="s">
@@ -7112,7 +7091,7 @@
         <v>64</v>
       </c>
       <c r="N48" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O48" s="11" t="s">
         <v>94</v>
@@ -7120,13 +7099,14 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="48">
-        <v>2.3199999999999999E-8</v>
+        <v>99</v>
+      </c>
+      <c r="B49" s="46">
+        <f>B48</f>
+        <v>0.03</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>63</v>
@@ -7159,7 +7139,7 @@
         <v>64</v>
       </c>
       <c r="N49" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O49" s="11" t="s">
         <v>94</v>
@@ -7167,139 +7147,186 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="48">
+        <v>2.3199999999999999E-8</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M50" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N50" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="48">
+      <c r="B51" s="48">
         <f>Hypothesis!D49</f>
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F50" s="13" t="s">
+      <c r="E51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="G51" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M50" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N50" s="13" t="s">
+      <c r="H51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N51" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+    <row r="52" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="43" t="s">
         <v>355</v>
       </c>
-      <c r="B51" s="46">
+      <c r="B52" s="46">
         <f>Hypothesis!D64</f>
         <v>0.15</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C52" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D52" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="35" t="s">
+      <c r="E52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F52" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="G52" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="H51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="I51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="J51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="K51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="L51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="M51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="N51" s="35" t="s">
+      <c r="H52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="L52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="M52" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="N52" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="O51" s="45"/>
-    </row>
-    <row r="52" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="O52" s="45"/>
+    </row>
+    <row r="53" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="47">
+      <c r="B53" s="47">
         <v>1</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C53" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D53" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" s="23" t="s">
+      <c r="E53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G52" s="23" t="s">
+      <c r="G53" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="H52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="I52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M52" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N52" s="23" t="s">
+      <c r="H53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M53" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N53" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="O52" s="24"/>
+      <c r="O53" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11610,7 +11637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E1620C-AF18-4A30-94EC-3B2E34B9A5F9}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -15517,7 +15544,7 @@
         <v>141</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -15613,7 +15640,7 @@
         <v>143</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -15661,7 +15688,7 @@
         <v>145</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -16599,1099 +16626,6 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30839250-B9B3-4863-A6E5-780C5AFC75AC}">
-  <dimension ref="A1:P31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="O1" s="11"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-    </row>
-    <row r="11" spans="1:16" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="P11" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="B12" s="40">
-        <v>-1</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="23" t="s">
-        <v>419</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="40">
-        <v>0</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O13" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="P13" s="24"/>
-    </row>
-    <row r="14" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="40">
-        <v>0</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O14" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="P14" s="24"/>
-    </row>
-    <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="40">
-        <v>0</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N15" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O15" s="23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="40">
-        <v>0</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O16" s="23" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="40">
-        <v>0</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O17" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="40">
-        <v>0</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O18" s="23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="B19" s="40">
-        <v>0</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O19" s="23" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="40">
-        <v>0</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O20" s="23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="B21" s="40">
-        <v>0</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O21" s="23" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="40">
-        <v>0</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N22" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O22" s="23" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="B23" s="40">
-        <v>0</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N23" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O23" s="23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="B24" s="40">
-        <v>0</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N24" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O24" s="23" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="B25" s="40">
-        <v>0</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O25" s="23" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="B26" s="40">
-        <v>0</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="40">
-        <v>0</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N27" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O27" s="23" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="B28" s="40">
-        <v>0</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O28" s="23" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>243</v>
-      </c>
-      <c r="B29" s="41">
-        <v>0</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="O29" s="13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>245</v>
-      </c>
-      <c r="B30" s="41">
-        <v>0</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="O30" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B31" s="40">
-        <v>1</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="M31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="O31" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="P31" s="24"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FCD044-1303-4FAB-83D7-76584F0D9B93}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -17935,12 +16869,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BCB970-6F91-449A-9CC2-6AEDC854A771}">
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18889,7 +17823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC13877F-C8AC-4C8A-A09F-523EF1E5A40E}">
   <dimension ref="A1:O15"/>
   <sheetViews>
@@ -19228,12 +18162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A789A5BF-8683-4EE3-8B60-10FBF3DEB298}">
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19388,7 +18322,7 @@
         <v>62</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>63</v>
@@ -19435,7 +18369,7 @@
         <v>246</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>63</v>
@@ -19522,12 +18456,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28F3D49-74C2-4BFC-A6B6-5745C01BC058}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20421,6 +19355,392 @@
         <v>401</v>
       </c>
       <c r="P27" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30839250-B9B3-4863-A6E5-780C5AFC75AC}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="1:16" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="40">
+        <v>1</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="P12" s="24"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="41">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="41">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" s="40">
+        <v>1</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="P15" s="24"/>
+    </row>
+    <row r="16" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="B16" s="40">
+        <v>1</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>401</v>
+      </c>
+      <c r="P16" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>